<commit_message>
modify template for indent
</commit_message>
<xml_diff>
--- a/web/material/template/indent_summary_template.xlsx
+++ b/web/material/template/indent_summary_template.xlsx
@@ -5,16 +5,16 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunshine/Documents/Itellij/Selling/web/material/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunshine/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10240" yWindow="3280" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="5000" yWindow="9280" windowWidth="28160" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>订货日期</t>
     <rPh sb="0" eb="1">
@@ -36,13 +36,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>订货人</t>
-    <rPh sb="0" eb="1">
-      <t>ding huo r</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>联系方式</t>
     <rPh sb="0" eb="1">
       <t>lian xi fang s</t>
@@ -67,16 +60,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>产品数量</t>
-    <rPh sb="0" eb="1">
-      <t>chan p</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>shu l</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>货款合计</t>
     <rPh sb="0" eb="1">
       <t>huo k</t>
@@ -105,25 +88,69 @@
   </si>
   <si>
     <t>代理商</t>
+  </si>
+  <si>
+    <t>顾客</t>
+    <rPh sb="0" eb="1">
+      <t>ding huo r</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数量</t>
+    <rPh sb="0" eb="1">
+      <t>chan pshu l</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单价</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发货日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>订单统计表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -136,7 +163,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -144,18 +171,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -210,7 +265,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -245,7 +300,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -430,48 +485,364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="46.83203125" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implementation of me center
</commit_message>
<xml_diff>
--- a/web/material/template/indent_summary_template.xlsx
+++ b/web/material/template/indent_summary_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunshine/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunshine/Documents/Itellij/Selling/web/material/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5000" yWindow="9280" windowWidth="28160" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="3860" yWindow="4140" windowWidth="28160" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>订货日期</t>
     <rPh sb="0" eb="1">
@@ -113,6 +113,13 @@
   </si>
   <si>
     <t>订单统计表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <rPh sb="0" eb="1">
+      <t>lei xing</t>
+    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -204,10 +211,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -485,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -503,23 +510,24 @@
     <col min="9" max="9" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="42" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -554,292 +562,315 @@
         <v>11</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>